<commit_message>
update of test references
</commit_message>
<xml_diff>
--- a/test/reference/from_sym/test.xlsx
+++ b/test/reference/from_sym/test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3492" uniqueCount="423">
   <si>
     <t>ID</t>
   </si>
@@ -1753,6 +1753,9 @@
       <c r="J2" s="2">
         <v>2</v>
       </c>
+      <c r="K2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1792,6 +1795,9 @@
       <c r="J3" s="3">
         <v>2</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L3" s="3" t="s">
         <v>22</v>
       </c>
@@ -1831,6 +1837,9 @@
       <c r="J4" s="3">
         <v>2</v>
       </c>
+      <c r="K4" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L4" s="3" t="s">
         <v>22</v>
       </c>
@@ -1870,6 +1879,9 @@
       <c r="J5" s="3">
         <v>2</v>
       </c>
+      <c r="K5" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1909,6 +1921,9 @@
       <c r="J6" s="4">
         <v>2</v>
       </c>
+      <c r="K6" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L6" s="4" t="s">
         <v>22</v>
       </c>
@@ -1948,6 +1963,9 @@
       <c r="J7" s="3">
         <v>2</v>
       </c>
+      <c r="K7" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1987,6 +2005,9 @@
       <c r="J8" s="3">
         <v>2</v>
       </c>
+      <c r="K8" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L8" s="3" t="s">
         <v>22</v>
       </c>
@@ -2026,6 +2047,9 @@
       <c r="J9" s="3">
         <v>2</v>
       </c>
+      <c r="K9" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L9" s="3" t="s">
         <v>22</v>
       </c>
@@ -2065,6 +2089,9 @@
       <c r="J10" s="4">
         <v>2</v>
       </c>
+      <c r="K10" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L10" s="4" t="s">
         <v>22</v>
       </c>
@@ -2104,6 +2131,9 @@
       <c r="J11" s="3">
         <v>2</v>
       </c>
+      <c r="K11" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L11" s="3" t="s">
         <v>22</v>
       </c>
@@ -2143,6 +2173,9 @@
       <c r="J12" s="3">
         <v>2</v>
       </c>
+      <c r="K12" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2182,6 +2215,9 @@
       <c r="J13" s="3">
         <v>2</v>
       </c>
+      <c r="K13" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L13" s="3" t="s">
         <v>22</v>
       </c>
@@ -2221,6 +2257,9 @@
       <c r="J14" s="4">
         <v>2</v>
       </c>
+      <c r="K14" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L14" s="4" t="s">
         <v>22</v>
       </c>
@@ -2260,6 +2299,9 @@
       <c r="J15" s="3">
         <v>2</v>
       </c>
+      <c r="K15" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L15" s="3" t="s">
         <v>22</v>
       </c>
@@ -2299,6 +2341,9 @@
       <c r="J16" s="3">
         <v>2</v>
       </c>
+      <c r="K16" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L16" s="3" t="s">
         <v>22</v>
       </c>
@@ -2338,6 +2383,9 @@
       <c r="J17" s="3">
         <v>2</v>
       </c>
+      <c r="K17" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L17" s="3" t="s">
         <v>22</v>
       </c>
@@ -2377,6 +2425,9 @@
       <c r="J18" s="4">
         <v>2</v>
       </c>
+      <c r="K18" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L18" s="4" t="s">
         <v>22</v>
       </c>
@@ -2416,6 +2467,9 @@
       <c r="J19" s="3">
         <v>2</v>
       </c>
+      <c r="K19" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L19" s="3" t="s">
         <v>22</v>
       </c>
@@ -2455,6 +2509,9 @@
       <c r="J20" s="3">
         <v>2</v>
       </c>
+      <c r="K20" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L20" s="3" t="s">
         <v>22</v>
       </c>
@@ -2494,6 +2551,9 @@
       <c r="J21" s="3">
         <v>2</v>
       </c>
+      <c r="K21" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L21" s="3" t="s">
         <v>22</v>
       </c>
@@ -2533,6 +2593,9 @@
       <c r="J22" s="4">
         <v>2</v>
       </c>
+      <c r="K22" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L22" s="4" t="s">
         <v>22</v>
       </c>
@@ -2572,6 +2635,9 @@
       <c r="J23" s="3">
         <v>2</v>
       </c>
+      <c r="K23" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L23" s="3" t="s">
         <v>22</v>
       </c>
@@ -2611,6 +2677,9 @@
       <c r="J24" s="3">
         <v>2</v>
       </c>
+      <c r="K24" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L24" s="3" t="s">
         <v>22</v>
       </c>
@@ -2650,6 +2719,9 @@
       <c r="J25" s="3">
         <v>2</v>
       </c>
+      <c r="K25" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L25" s="3" t="s">
         <v>22</v>
       </c>
@@ -2689,6 +2761,9 @@
       <c r="J26" s="4">
         <v>2</v>
       </c>
+      <c r="K26" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L26" s="4" t="s">
         <v>22</v>
       </c>
@@ -2728,6 +2803,9 @@
       <c r="J27" s="3">
         <v>2</v>
       </c>
+      <c r="K27" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L27" s="3" t="s">
         <v>22</v>
       </c>
@@ -2767,6 +2845,9 @@
       <c r="J28" s="3">
         <v>2</v>
       </c>
+      <c r="K28" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L28" s="3" t="s">
         <v>22</v>
       </c>
@@ -2806,6 +2887,9 @@
       <c r="J29" s="3">
         <v>2</v>
       </c>
+      <c r="K29" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L29" s="3" t="s">
         <v>22</v>
       </c>
@@ -2845,6 +2929,9 @@
       <c r="J30" s="4">
         <v>2</v>
       </c>
+      <c r="K30" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L30" s="4" t="s">
         <v>22</v>
       </c>
@@ -2884,6 +2971,9 @@
       <c r="J31" s="3">
         <v>2</v>
       </c>
+      <c r="K31" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L31" s="3" t="s">
         <v>22</v>
       </c>
@@ -2923,6 +3013,9 @@
       <c r="J32" s="3">
         <v>2</v>
       </c>
+      <c r="K32" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L32" s="3" t="s">
         <v>22</v>
       </c>
@@ -2962,6 +3055,9 @@
       <c r="J33" s="3">
         <v>2</v>
       </c>
+      <c r="K33" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L33" s="3" t="s">
         <v>22</v>
       </c>
@@ -3001,6 +3097,9 @@
       <c r="J34" s="4">
         <v>2</v>
       </c>
+      <c r="K34" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L34" s="4" t="s">
         <v>22</v>
       </c>
@@ -3040,6 +3139,9 @@
       <c r="J35" s="3">
         <v>2</v>
       </c>
+      <c r="K35" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L35" s="3" t="s">
         <v>22</v>
       </c>
@@ -3079,6 +3181,9 @@
       <c r="J36" s="3">
         <v>2</v>
       </c>
+      <c r="K36" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L36" s="3" t="s">
         <v>22</v>
       </c>
@@ -3118,6 +3223,9 @@
       <c r="J37" s="3">
         <v>2</v>
       </c>
+      <c r="K37" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L37" s="3" t="s">
         <v>22</v>
       </c>
@@ -3157,6 +3265,9 @@
       <c r="J38" s="4">
         <v>2</v>
       </c>
+      <c r="K38" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L38" s="4" t="s">
         <v>22</v>
       </c>
@@ -3196,6 +3307,9 @@
       <c r="J39" s="3">
         <v>2</v>
       </c>
+      <c r="K39" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L39" s="3" t="s">
         <v>22</v>
       </c>
@@ -3235,6 +3349,9 @@
       <c r="J40" s="3">
         <v>2</v>
       </c>
+      <c r="K40" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L40" s="3" t="s">
         <v>22</v>
       </c>
@@ -3274,6 +3391,9 @@
       <c r="J41" s="3">
         <v>2</v>
       </c>
+      <c r="K41" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L41" s="3" t="s">
         <v>22</v>
       </c>
@@ -3313,6 +3433,9 @@
       <c r="J42" s="4">
         <v>2</v>
       </c>
+      <c r="K42" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L42" s="4" t="s">
         <v>22</v>
       </c>
@@ -3352,6 +3475,9 @@
       <c r="J43" s="3">
         <v>2</v>
       </c>
+      <c r="K43" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L43" s="3" t="s">
         <v>22</v>
       </c>
@@ -3391,6 +3517,9 @@
       <c r="J44" s="3">
         <v>2</v>
       </c>
+      <c r="K44" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L44" s="3" t="s">
         <v>22</v>
       </c>
@@ -3430,6 +3559,9 @@
       <c r="J45" s="3">
         <v>2</v>
       </c>
+      <c r="K45" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L45" s="3" t="s">
         <v>22</v>
       </c>
@@ -3469,6 +3601,9 @@
       <c r="J46" s="2">
         <v>2</v>
       </c>
+      <c r="K46" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L46" s="2" t="s">
         <v>22</v>
       </c>
@@ -3508,6 +3643,9 @@
       <c r="J47" s="3">
         <v>2</v>
       </c>
+      <c r="K47" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L47" s="3" t="s">
         <v>22</v>
       </c>
@@ -3547,6 +3685,9 @@
       <c r="J48" s="3">
         <v>2</v>
       </c>
+      <c r="K48" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L48" s="3" t="s">
         <v>22</v>
       </c>
@@ -3586,6 +3727,9 @@
       <c r="J49" s="3">
         <v>2</v>
       </c>
+      <c r="K49" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L49" s="3" t="s">
         <v>22</v>
       </c>
@@ -3625,6 +3769,9 @@
       <c r="J50" s="4">
         <v>2</v>
       </c>
+      <c r="K50" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L50" s="4" t="s">
         <v>22</v>
       </c>
@@ -3664,6 +3811,9 @@
       <c r="J51" s="3">
         <v>2</v>
       </c>
+      <c r="K51" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L51" s="3" t="s">
         <v>22</v>
       </c>
@@ -3703,6 +3853,9 @@
       <c r="J52" s="3">
         <v>2</v>
       </c>
+      <c r="K52" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L52" s="3" t="s">
         <v>22</v>
       </c>
@@ -3742,6 +3895,9 @@
       <c r="J53" s="3">
         <v>2</v>
       </c>
+      <c r="K53" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L53" s="3" t="s">
         <v>22</v>
       </c>
@@ -3781,6 +3937,9 @@
       <c r="J54" s="4">
         <v>2</v>
       </c>
+      <c r="K54" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L54" s="4" t="s">
         <v>22</v>
       </c>
@@ -3820,6 +3979,9 @@
       <c r="J55" s="3">
         <v>2</v>
       </c>
+      <c r="K55" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L55" s="3" t="s">
         <v>22</v>
       </c>
@@ -3859,6 +4021,9 @@
       <c r="J56" s="3">
         <v>2</v>
       </c>
+      <c r="K56" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L56" s="3" t="s">
         <v>22</v>
       </c>
@@ -3898,6 +4063,9 @@
       <c r="J57" s="3">
         <v>2</v>
       </c>
+      <c r="K57" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L57" s="3" t="s">
         <v>22</v>
       </c>
@@ -3937,6 +4105,9 @@
       <c r="J58" s="4">
         <v>2</v>
       </c>
+      <c r="K58" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L58" s="4" t="s">
         <v>22</v>
       </c>
@@ -3976,6 +4147,9 @@
       <c r="J59" s="3">
         <v>2</v>
       </c>
+      <c r="K59" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L59" s="3" t="s">
         <v>22</v>
       </c>
@@ -4015,6 +4189,9 @@
       <c r="J60" s="3">
         <v>2</v>
       </c>
+      <c r="K60" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L60" s="3" t="s">
         <v>22</v>
       </c>
@@ -4054,6 +4231,9 @@
       <c r="J61" s="3">
         <v>2</v>
       </c>
+      <c r="K61" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L61" s="3" t="s">
         <v>22</v>
       </c>
@@ -4093,6 +4273,9 @@
       <c r="J62" s="4">
         <v>2</v>
       </c>
+      <c r="K62" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L62" s="4" t="s">
         <v>22</v>
       </c>
@@ -4132,6 +4315,9 @@
       <c r="J63" s="3">
         <v>2</v>
       </c>
+      <c r="K63" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L63" s="3" t="s">
         <v>22</v>
       </c>
@@ -4171,6 +4357,9 @@
       <c r="J64" s="3">
         <v>2</v>
       </c>
+      <c r="K64" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L64" s="3" t="s">
         <v>22</v>
       </c>
@@ -4210,6 +4399,9 @@
       <c r="J65" s="3">
         <v>2</v>
       </c>
+      <c r="K65" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L65" s="3" t="s">
         <v>22</v>
       </c>
@@ -4249,6 +4441,9 @@
       <c r="J66" s="4">
         <v>2</v>
       </c>
+      <c r="K66" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L66" s="4" t="s">
         <v>22</v>
       </c>
@@ -4288,6 +4483,9 @@
       <c r="J67" s="3">
         <v>2</v>
       </c>
+      <c r="K67" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L67" s="3" t="s">
         <v>22</v>
       </c>
@@ -4327,6 +4525,9 @@
       <c r="J68" s="3">
         <v>2</v>
       </c>
+      <c r="K68" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L68" s="3" t="s">
         <v>22</v>
       </c>
@@ -4366,6 +4567,9 @@
       <c r="J69" s="3">
         <v>2</v>
       </c>
+      <c r="K69" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L69" s="3" t="s">
         <v>22</v>
       </c>
@@ -4405,6 +4609,9 @@
       <c r="J70" s="4">
         <v>2</v>
       </c>
+      <c r="K70" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L70" s="4" t="s">
         <v>22</v>
       </c>
@@ -4444,6 +4651,9 @@
       <c r="J71" s="3">
         <v>2</v>
       </c>
+      <c r="K71" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L71" s="3" t="s">
         <v>22</v>
       </c>
@@ -4483,6 +4693,9 @@
       <c r="J72" s="3">
         <v>2</v>
       </c>
+      <c r="K72" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L72" s="3" t="s">
         <v>22</v>
       </c>
@@ -4522,6 +4735,9 @@
       <c r="J73" s="3">
         <v>2</v>
       </c>
+      <c r="K73" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L73" s="3" t="s">
         <v>22</v>
       </c>
@@ -4561,6 +4777,9 @@
       <c r="J74" s="4">
         <v>2</v>
       </c>
+      <c r="K74" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L74" s="4" t="s">
         <v>22</v>
       </c>
@@ -4600,6 +4819,9 @@
       <c r="J75" s="3">
         <v>2</v>
       </c>
+      <c r="K75" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L75" s="3" t="s">
         <v>22</v>
       </c>
@@ -4639,6 +4861,9 @@
       <c r="J76" s="3">
         <v>2</v>
       </c>
+      <c r="K76" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L76" s="3" t="s">
         <v>22</v>
       </c>
@@ -4678,6 +4903,9 @@
       <c r="J77" s="3">
         <v>2</v>
       </c>
+      <c r="K77" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L77" s="3" t="s">
         <v>22</v>
       </c>
@@ -4717,6 +4945,9 @@
       <c r="J78" s="4">
         <v>2</v>
       </c>
+      <c r="K78" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L78" s="4" t="s">
         <v>22</v>
       </c>
@@ -4756,6 +4987,9 @@
       <c r="J79" s="3">
         <v>2</v>
       </c>
+      <c r="K79" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L79" s="3" t="s">
         <v>22</v>
       </c>
@@ -4795,6 +5029,9 @@
       <c r="J80" s="3">
         <v>2</v>
       </c>
+      <c r="K80" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L80" s="3" t="s">
         <v>22</v>
       </c>
@@ -4834,6 +5071,9 @@
       <c r="J81" s="3">
         <v>2</v>
       </c>
+      <c r="K81" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L81" s="3" t="s">
         <v>22</v>
       </c>
@@ -4873,6 +5113,9 @@
       <c r="J82" s="4">
         <v>2</v>
       </c>
+      <c r="K82" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L82" s="4" t="s">
         <v>22</v>
       </c>
@@ -4912,6 +5155,9 @@
       <c r="J83" s="3">
         <v>2</v>
       </c>
+      <c r="K83" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L83" s="3" t="s">
         <v>22</v>
       </c>
@@ -4951,6 +5197,9 @@
       <c r="J84" s="3">
         <v>2</v>
       </c>
+      <c r="K84" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L84" s="3" t="s">
         <v>22</v>
       </c>
@@ -4990,6 +5239,9 @@
       <c r="J85" s="3">
         <v>2</v>
       </c>
+      <c r="K85" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L85" s="3" t="s">
         <v>22</v>
       </c>
@@ -5029,6 +5281,9 @@
       <c r="J86" s="4">
         <v>2</v>
       </c>
+      <c r="K86" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L86" s="4" t="s">
         <v>22</v>
       </c>
@@ -5068,6 +5323,9 @@
       <c r="J87" s="3">
         <v>2</v>
       </c>
+      <c r="K87" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L87" s="3" t="s">
         <v>22</v>
       </c>
@@ -5107,6 +5365,9 @@
       <c r="J88" s="3">
         <v>2</v>
       </c>
+      <c r="K88" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L88" s="3" t="s">
         <v>22</v>
       </c>
@@ -5146,6 +5407,9 @@
       <c r="J89" s="3">
         <v>2</v>
       </c>
+      <c r="K89" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L89" s="3" t="s">
         <v>22</v>
       </c>
@@ -5185,6 +5449,9 @@
       <c r="J90" s="2">
         <v>32</v>
       </c>
+      <c r="K90" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L90" s="2" t="s">
         <v>22</v>
       </c>
@@ -5224,6 +5491,9 @@
       <c r="J91" s="4">
         <v>32</v>
       </c>
+      <c r="K91" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L91" s="4" t="s">
         <v>22</v>
       </c>
@@ -5263,6 +5533,9 @@
       <c r="J92" s="2">
         <v>16</v>
       </c>
+      <c r="K92" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L92" s="2" t="s">
         <v>22</v>
       </c>
@@ -5302,6 +5575,9 @@
       <c r="J93" s="4">
         <v>16</v>
       </c>
+      <c r="K93" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L93" s="4" t="s">
         <v>22</v>
       </c>
@@ -5761,6 +6037,9 @@
       <c r="J104" s="4">
         <v>16</v>
       </c>
+      <c r="K104" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L104" s="4" t="s">
         <v>22</v>
       </c>
@@ -5798,6 +6077,9 @@
       <c r="J105" s="4">
         <v>16</v>
       </c>
+      <c r="K105" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L105" s="4" t="s">
         <v>22</v>
       </c>
@@ -5837,6 +6119,9 @@
       <c r="J106" s="4">
         <v>16</v>
       </c>
+      <c r="K106" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L106" s="4" t="s">
         <v>22</v>
       </c>
@@ -5876,6 +6161,9 @@
       <c r="J107" s="4">
         <v>16</v>
       </c>
+      <c r="K107" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L107" s="4" t="s">
         <v>22</v>
       </c>
@@ -5915,6 +6203,9 @@
       <c r="J108" s="4">
         <v>16</v>
       </c>
+      <c r="K108" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L108" s="4" t="s">
         <v>22</v>
       </c>
@@ -5954,6 +6245,9 @@
       <c r="J109" s="4">
         <v>16</v>
       </c>
+      <c r="K109" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L109" s="4" t="s">
         <v>22</v>
       </c>
@@ -5993,6 +6287,9 @@
       <c r="J110" s="4">
         <v>8</v>
       </c>
+      <c r="K110" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L110" s="4" t="s">
         <v>22</v>
       </c>
@@ -6030,6 +6327,9 @@
       <c r="J111" s="4">
         <v>16</v>
       </c>
+      <c r="K111" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L111" s="4" t="s">
         <v>22</v>
       </c>
@@ -6067,6 +6367,9 @@
       <c r="J112" s="4">
         <v>16</v>
       </c>
+      <c r="K112" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L112" s="4" t="s">
         <v>22</v>
       </c>
@@ -6106,6 +6409,9 @@
       <c r="J113" s="4">
         <v>2</v>
       </c>
+      <c r="K113" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L113" s="4" t="s">
         <v>22</v>
       </c>
@@ -6145,6 +6451,9 @@
       <c r="J114" s="3">
         <v>2</v>
       </c>
+      <c r="K114" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L114" s="3" t="s">
         <v>22</v>
       </c>
@@ -6184,6 +6493,9 @@
       <c r="J115" s="3">
         <v>2</v>
       </c>
+      <c r="K115" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L115" s="3" t="s">
         <v>22</v>
       </c>
@@ -6223,6 +6535,9 @@
       <c r="J116" s="3">
         <v>2</v>
       </c>
+      <c r="K116" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L116" s="3" t="s">
         <v>22</v>
       </c>
@@ -6262,6 +6577,9 @@
       <c r="J117" s="4">
         <v>8</v>
       </c>
+      <c r="K117" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L117" s="4" t="s">
         <v>22</v>
       </c>
@@ -6299,6 +6617,9 @@
       <c r="J118" s="4">
         <v>4</v>
       </c>
+      <c r="K118" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L118" s="4" t="s">
         <v>22</v>
       </c>
@@ -6338,6 +6659,9 @@
       <c r="J119" s="3">
         <v>4</v>
       </c>
+      <c r="K119" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L119" s="3" t="s">
         <v>22</v>
       </c>
@@ -6377,6 +6701,9 @@
       <c r="J120" s="3">
         <v>4</v>
       </c>
+      <c r="K120" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L120" s="3" t="s">
         <v>22</v>
       </c>
@@ -6416,6 +6743,9 @@
       <c r="J121" s="3">
         <v>4</v>
       </c>
+      <c r="K121" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L121" s="3" t="s">
         <v>22</v>
       </c>
@@ -6455,6 +6785,9 @@
       <c r="J122" s="4">
         <v>16</v>
       </c>
+      <c r="K122" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L122" s="4" t="s">
         <v>22</v>
       </c>
@@ -6494,6 +6827,9 @@
       <c r="J123" s="4">
         <v>16</v>
       </c>
+      <c r="K123" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L123" s="4" t="s">
         <v>22</v>
       </c>
@@ -6533,6 +6869,9 @@
       <c r="J124" s="4">
         <v>16</v>
       </c>
+      <c r="K124" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L124" s="4" t="s">
         <v>22</v>
       </c>
@@ -6572,6 +6911,9 @@
       <c r="J125" s="4">
         <v>16</v>
       </c>
+      <c r="K125" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L125" s="4" t="s">
         <v>22</v>
       </c>
@@ -6611,6 +6953,9 @@
       <c r="J126" s="4">
         <v>16</v>
       </c>
+      <c r="K126" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L126" s="4" t="s">
         <v>22</v>
       </c>
@@ -6650,6 +6995,9 @@
       <c r="J127" s="4">
         <v>16</v>
       </c>
+      <c r="K127" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L127" s="4" t="s">
         <v>22</v>
       </c>
@@ -6689,6 +7037,9 @@
       <c r="J128" s="4">
         <v>16</v>
       </c>
+      <c r="K128" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L128" s="4" t="s">
         <v>22</v>
       </c>
@@ -6728,6 +7079,9 @@
       <c r="J129" s="4">
         <v>16</v>
       </c>
+      <c r="K129" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L129" s="4" t="s">
         <v>22</v>
       </c>
@@ -6767,6 +7121,9 @@
       <c r="J130" s="4">
         <v>16</v>
       </c>
+      <c r="K130" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L130" s="4" t="s">
         <v>22</v>
       </c>
@@ -6804,6 +7161,9 @@
       <c r="J131" s="4">
         <v>16</v>
       </c>
+      <c r="K131" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L131" s="4" t="s">
         <v>22</v>
       </c>
@@ -6843,6 +7203,9 @@
       <c r="J132" s="2">
         <v>32</v>
       </c>
+      <c r="K132" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L132" s="2" t="s">
         <v>22</v>
       </c>
@@ -6882,6 +7245,9 @@
       <c r="J133" s="4">
         <v>32</v>
       </c>
+      <c r="K133" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L133" s="4" t="s">
         <v>22</v>
       </c>
@@ -6921,6 +7287,9 @@
       <c r="J134" s="2">
         <v>16</v>
       </c>
+      <c r="K134" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L134" s="2" t="s">
         <v>22</v>
       </c>
@@ -6960,6 +7329,9 @@
       <c r="J135" s="4">
         <v>16</v>
       </c>
+      <c r="K135" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L135" s="4" t="s">
         <v>22</v>
       </c>
@@ -6997,6 +7369,9 @@
       <c r="J136" s="2">
         <v>2</v>
       </c>
+      <c r="K136" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L136" s="2" t="s">
         <v>22</v>
       </c>
@@ -7034,6 +7409,9 @@
       <c r="J137" s="3">
         <v>2</v>
       </c>
+      <c r="K137" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L137" s="3" t="s">
         <v>22</v>
       </c>
@@ -7071,6 +7449,9 @@
       <c r="J138" s="3">
         <v>2</v>
       </c>
+      <c r="K138" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L138" s="3" t="s">
         <v>22</v>
       </c>
@@ -7108,6 +7489,9 @@
       <c r="J139" s="3">
         <v>2</v>
       </c>
+      <c r="K139" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L139" s="3" t="s">
         <v>22</v>
       </c>
@@ -7145,6 +7529,9 @@
       <c r="J140" s="4">
         <v>16</v>
       </c>
+      <c r="K140" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L140" s="4" t="s">
         <v>22</v>
       </c>
@@ -7180,6 +7567,9 @@
       <c r="J141" s="4">
         <v>32</v>
       </c>
+      <c r="K141" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L141" s="4" t="s">
         <v>22</v>
       </c>
@@ -7219,6 +7609,9 @@
       <c r="J142" s="2">
         <v>16</v>
       </c>
+      <c r="K142" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L142" s="2" t="s">
         <v>22</v>
       </c>
@@ -7260,6 +7653,9 @@
       <c r="J143" s="4">
         <v>16</v>
       </c>
+      <c r="K143" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L143" s="4" t="s">
         <v>22</v>
       </c>
@@ -7301,6 +7697,9 @@
       <c r="J144" s="4">
         <v>16</v>
       </c>
+      <c r="K144" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L144" s="4" t="s">
         <v>22</v>
       </c>
@@ -7342,6 +7741,9 @@
       <c r="J145" s="2">
         <v>2</v>
       </c>
+      <c r="K145" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L145" s="2" t="s">
         <v>22</v>
       </c>
@@ -7383,6 +7785,9 @@
       <c r="J146" s="3">
         <v>2</v>
       </c>
+      <c r="K146" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L146" s="3" t="s">
         <v>22</v>
       </c>
@@ -7424,6 +7829,9 @@
       <c r="J147" s="3">
         <v>2</v>
       </c>
+      <c r="K147" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L147" s="3" t="s">
         <v>22</v>
       </c>
@@ -7465,6 +7873,9 @@
       <c r="J148" s="3">
         <v>2</v>
       </c>
+      <c r="K148" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L148" s="3" t="s">
         <v>22</v>
       </c>
@@ -7506,6 +7917,9 @@
       <c r="J149" s="4">
         <v>2</v>
       </c>
+      <c r="K149" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L149" s="4" t="s">
         <v>22</v>
       </c>
@@ -7547,6 +7961,9 @@
       <c r="J150" s="3">
         <v>2</v>
       </c>
+      <c r="K150" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L150" s="3" t="s">
         <v>22</v>
       </c>
@@ -7588,6 +8005,9 @@
       <c r="J151" s="3">
         <v>2</v>
       </c>
+      <c r="K151" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L151" s="3" t="s">
         <v>22</v>
       </c>
@@ -7629,6 +8049,9 @@
       <c r="J152" s="3">
         <v>2</v>
       </c>
+      <c r="K152" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L152" s="3" t="s">
         <v>22</v>
       </c>
@@ -7670,6 +8093,9 @@
       <c r="J153" s="4">
         <v>4</v>
       </c>
+      <c r="K153" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L153" s="4" t="s">
         <v>22</v>
       </c>
@@ -7711,6 +8137,9 @@
       <c r="J154" s="3">
         <v>4</v>
       </c>
+      <c r="K154" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L154" s="3" t="s">
         <v>22</v>
       </c>
@@ -7752,6 +8181,9 @@
       <c r="J155" s="3">
         <v>4</v>
       </c>
+      <c r="K155" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L155" s="3" t="s">
         <v>22</v>
       </c>
@@ -7793,6 +8225,9 @@
       <c r="J156" s="3">
         <v>4</v>
       </c>
+      <c r="K156" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L156" s="3" t="s">
         <v>22</v>
       </c>
@@ -7834,6 +8269,9 @@
       <c r="J157" s="3">
         <v>4</v>
       </c>
+      <c r="K157" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L157" s="3" t="s">
         <v>22</v>
       </c>
@@ -7875,6 +8313,9 @@
       <c r="J158" s="3">
         <v>4</v>
       </c>
+      <c r="K158" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L158" s="3" t="s">
         <v>22</v>
       </c>
@@ -7916,6 +8357,9 @@
       <c r="J159" s="3">
         <v>4</v>
       </c>
+      <c r="K159" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L159" s="3" t="s">
         <v>22</v>
       </c>
@@ -7957,6 +8401,9 @@
       <c r="J160" s="3">
         <v>4</v>
       </c>
+      <c r="K160" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L160" s="3" t="s">
         <v>22</v>
       </c>
@@ -7998,6 +8445,9 @@
       <c r="J161" s="3">
         <v>4</v>
       </c>
+      <c r="K161" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L161" s="3" t="s">
         <v>22</v>
       </c>
@@ -8039,6 +8489,9 @@
       <c r="J162" s="3">
         <v>4</v>
       </c>
+      <c r="K162" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L162" s="3" t="s">
         <v>22</v>
       </c>
@@ -8080,6 +8533,9 @@
       <c r="J163" s="3">
         <v>4</v>
       </c>
+      <c r="K163" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L163" s="3" t="s">
         <v>22</v>
       </c>
@@ -8121,6 +8577,9 @@
       <c r="J164" s="3">
         <v>4</v>
       </c>
+      <c r="K164" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L164" s="3" t="s">
         <v>22</v>
       </c>
@@ -8162,6 +8621,9 @@
       <c r="J165" s="3">
         <v>4</v>
       </c>
+      <c r="K165" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L165" s="3" t="s">
         <v>22</v>
       </c>
@@ -8203,6 +8665,9 @@
       <c r="J166" s="3">
         <v>4</v>
       </c>
+      <c r="K166" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L166" s="3" t="s">
         <v>22</v>
       </c>
@@ -8244,6 +8709,9 @@
       <c r="J167" s="3">
         <v>4</v>
       </c>
+      <c r="K167" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L167" s="3" t="s">
         <v>22</v>
       </c>
@@ -8285,6 +8753,9 @@
       <c r="J168" s="3">
         <v>4</v>
       </c>
+      <c r="K168" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L168" s="3" t="s">
         <v>22</v>
       </c>
@@ -8326,6 +8797,9 @@
       <c r="J169" s="4">
         <v>2</v>
       </c>
+      <c r="K169" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L169" s="4" t="s">
         <v>22</v>
       </c>
@@ -8367,6 +8841,9 @@
       <c r="J170" s="3">
         <v>2</v>
       </c>
+      <c r="K170" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L170" s="3" t="s">
         <v>22</v>
       </c>
@@ -8408,6 +8885,9 @@
       <c r="J171" s="3">
         <v>2</v>
       </c>
+      <c r="K171" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L171" s="3" t="s">
         <v>22</v>
       </c>
@@ -8449,6 +8929,9 @@
       <c r="J172" s="3">
         <v>2</v>
       </c>
+      <c r="K172" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L172" s="3" t="s">
         <v>22</v>
       </c>
@@ -8490,6 +8973,9 @@
       <c r="J173" s="4">
         <v>2</v>
       </c>
+      <c r="K173" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L173" s="4" t="s">
         <v>22</v>
       </c>
@@ -8531,6 +9017,9 @@
       <c r="J174" s="3">
         <v>2</v>
       </c>
+      <c r="K174" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L174" s="3" t="s">
         <v>22</v>
       </c>
@@ -8572,6 +9061,9 @@
       <c r="J175" s="3">
         <v>2</v>
       </c>
+      <c r="K175" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L175" s="3" t="s">
         <v>22</v>
       </c>
@@ -8613,6 +9105,9 @@
       <c r="J176" s="3">
         <v>2</v>
       </c>
+      <c r="K176" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L176" s="3" t="s">
         <v>22</v>
       </c>
@@ -8654,6 +9149,9 @@
       <c r="J177" s="4">
         <v>2</v>
       </c>
+      <c r="K177" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L177" s="4" t="s">
         <v>22</v>
       </c>
@@ -8695,6 +9193,9 @@
       <c r="J178" s="3">
         <v>2</v>
       </c>
+      <c r="K178" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L178" s="3" t="s">
         <v>22</v>
       </c>
@@ -8736,6 +9237,9 @@
       <c r="J179" s="3">
         <v>2</v>
       </c>
+      <c r="K179" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L179" s="3" t="s">
         <v>22</v>
       </c>
@@ -8777,6 +9281,9 @@
       <c r="J180" s="3">
         <v>2</v>
       </c>
+      <c r="K180" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L180" s="3" t="s">
         <v>22</v>
       </c>
@@ -8818,6 +9325,9 @@
       <c r="J181" s="4">
         <v>2</v>
       </c>
+      <c r="K181" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L181" s="4" t="s">
         <v>22</v>
       </c>
@@ -8859,6 +9369,9 @@
       <c r="J182" s="3">
         <v>2</v>
       </c>
+      <c r="K182" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L182" s="3" t="s">
         <v>22</v>
       </c>
@@ -8900,6 +9413,9 @@
       <c r="J183" s="3">
         <v>2</v>
       </c>
+      <c r="K183" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L183" s="3" t="s">
         <v>22</v>
       </c>
@@ -8940,6 +9456,9 @@
       </c>
       <c r="J184" s="3">
         <v>2</v>
+      </c>
+      <c r="K184" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="L184" s="3" t="s">
         <v>22</v>
@@ -8982,6 +9501,9 @@
       <c r="J185" s="4">
         <v>2</v>
       </c>
+      <c r="K185" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L185" s="4" t="s">
         <v>22</v>
       </c>
@@ -9023,6 +9545,9 @@
       <c r="J186" s="3">
         <v>2</v>
       </c>
+      <c r="K186" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L186" s="3" t="s">
         <v>22</v>
       </c>
@@ -9064,6 +9589,9 @@
       <c r="J187" s="3">
         <v>2</v>
       </c>
+      <c r="K187" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L187" s="3" t="s">
         <v>22</v>
       </c>
@@ -9105,6 +9633,9 @@
       <c r="J188" s="3">
         <v>2</v>
       </c>
+      <c r="K188" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L188" s="3" t="s">
         <v>22</v>
       </c>
@@ -9146,6 +9677,9 @@
       <c r="J189" s="4">
         <v>2</v>
       </c>
+      <c r="K189" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L189" s="4" t="s">
         <v>22</v>
       </c>
@@ -9187,6 +9721,9 @@
       <c r="J190" s="3">
         <v>2</v>
       </c>
+      <c r="K190" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L190" s="3" t="s">
         <v>22</v>
       </c>
@@ -9228,6 +9765,9 @@
       <c r="J191" s="3">
         <v>2</v>
       </c>
+      <c r="K191" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L191" s="3" t="s">
         <v>22</v>
       </c>
@@ -9269,6 +9809,9 @@
       <c r="J192" s="3">
         <v>2</v>
       </c>
+      <c r="K192" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L192" s="3" t="s">
         <v>22</v>
       </c>
@@ -9310,6 +9853,9 @@
       <c r="J193" s="4">
         <v>2</v>
       </c>
+      <c r="K193" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L193" s="4" t="s">
         <v>22</v>
       </c>
@@ -9351,6 +9897,9 @@
       <c r="J194" s="3">
         <v>2</v>
       </c>
+      <c r="K194" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L194" s="3" t="s">
         <v>22</v>
       </c>
@@ -9392,6 +9941,9 @@
       <c r="J195" s="3">
         <v>2</v>
       </c>
+      <c r="K195" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L195" s="3" t="s">
         <v>22</v>
       </c>
@@ -9433,6 +9985,9 @@
       <c r="J196" s="3">
         <v>2</v>
       </c>
+      <c r="K196" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L196" s="3" t="s">
         <v>22</v>
       </c>
@@ -9474,6 +10029,9 @@
       <c r="J197" s="4">
         <v>2</v>
       </c>
+      <c r="K197" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L197" s="4" t="s">
         <v>22</v>
       </c>
@@ -9515,6 +10073,9 @@
       <c r="J198" s="3">
         <v>2</v>
       </c>
+      <c r="K198" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L198" s="3" t="s">
         <v>22</v>
       </c>
@@ -9556,6 +10117,9 @@
       <c r="J199" s="3">
         <v>2</v>
       </c>
+      <c r="K199" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L199" s="3" t="s">
         <v>22</v>
       </c>
@@ -9597,6 +10161,9 @@
       <c r="J200" s="3">
         <v>2</v>
       </c>
+      <c r="K200" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L200" s="3" t="s">
         <v>22</v>
       </c>
@@ -9638,6 +10205,9 @@
       <c r="J201" s="4">
         <v>2</v>
       </c>
+      <c r="K201" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L201" s="4" t="s">
         <v>22</v>
       </c>
@@ -9679,6 +10249,9 @@
       <c r="J202" s="3">
         <v>2</v>
       </c>
+      <c r="K202" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L202" s="3" t="s">
         <v>22</v>
       </c>
@@ -9720,6 +10293,9 @@
       <c r="J203" s="3">
         <v>2</v>
       </c>
+      <c r="K203" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L203" s="3" t="s">
         <v>22</v>
       </c>
@@ -9761,6 +10337,9 @@
       <c r="J204" s="3">
         <v>2</v>
       </c>
+      <c r="K204" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L204" s="3" t="s">
         <v>22</v>
       </c>
@@ -9802,6 +10381,9 @@
       <c r="J205" s="4">
         <v>2</v>
       </c>
+      <c r="K205" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L205" s="4" t="s">
         <v>22</v>
       </c>
@@ -9843,6 +10425,9 @@
       <c r="J206" s="3">
         <v>2</v>
       </c>
+      <c r="K206" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L206" s="3" t="s">
         <v>22</v>
       </c>
@@ -9884,6 +10469,9 @@
       <c r="J207" s="3">
         <v>2</v>
       </c>
+      <c r="K207" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L207" s="3" t="s">
         <v>22</v>
       </c>
@@ -9925,6 +10513,9 @@
       <c r="J208" s="3">
         <v>2</v>
       </c>
+      <c r="K208" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L208" s="3" t="s">
         <v>22</v>
       </c>
@@ -9966,6 +10557,9 @@
       <c r="J209" s="4">
         <v>2</v>
       </c>
+      <c r="K209" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L209" s="4" t="s">
         <v>22</v>
       </c>
@@ -10007,6 +10601,9 @@
       <c r="J210" s="3">
         <v>2</v>
       </c>
+      <c r="K210" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L210" s="3" t="s">
         <v>22</v>
       </c>
@@ -10048,6 +10645,9 @@
       <c r="J211" s="3">
         <v>2</v>
       </c>
+      <c r="K211" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L211" s="3" t="s">
         <v>22</v>
       </c>
@@ -10089,6 +10689,9 @@
       <c r="J212" s="3">
         <v>2</v>
       </c>
+      <c r="K212" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L212" s="3" t="s">
         <v>22</v>
       </c>
@@ -10130,6 +10733,9 @@
       <c r="J213" s="4">
         <v>2</v>
       </c>
+      <c r="K213" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L213" s="4" t="s">
         <v>22</v>
       </c>
@@ -10171,6 +10777,9 @@
       <c r="J214" s="3">
         <v>2</v>
       </c>
+      <c r="K214" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L214" s="3" t="s">
         <v>22</v>
       </c>
@@ -10212,6 +10821,9 @@
       <c r="J215" s="3">
         <v>2</v>
       </c>
+      <c r="K215" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L215" s="3" t="s">
         <v>22</v>
       </c>
@@ -10253,6 +10865,9 @@
       <c r="J216" s="3">
         <v>2</v>
       </c>
+      <c r="K216" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L216" s="3" t="s">
         <v>22</v>
       </c>
@@ -10294,6 +10909,9 @@
       <c r="J217" s="4">
         <v>2</v>
       </c>
+      <c r="K217" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L217" s="4" t="s">
         <v>22</v>
       </c>
@@ -10335,6 +10953,9 @@
       <c r="J218" s="3">
         <v>2</v>
       </c>
+      <c r="K218" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L218" s="3" t="s">
         <v>22</v>
       </c>
@@ -10376,6 +10997,9 @@
       <c r="J219" s="3">
         <v>2</v>
       </c>
+      <c r="K219" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L219" s="3" t="s">
         <v>22</v>
       </c>
@@ -10417,6 +11041,9 @@
       <c r="J220" s="3">
         <v>2</v>
       </c>
+      <c r="K220" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L220" s="3" t="s">
         <v>22</v>
       </c>
@@ -10458,6 +11085,9 @@
       <c r="J221" s="4">
         <v>2</v>
       </c>
+      <c r="K221" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L221" s="4" t="s">
         <v>22</v>
       </c>
@@ -10499,6 +11129,9 @@
       <c r="J222" s="3">
         <v>2</v>
       </c>
+      <c r="K222" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L222" s="3" t="s">
         <v>22</v>
       </c>
@@ -10540,6 +11173,9 @@
       <c r="J223" s="3">
         <v>2</v>
       </c>
+      <c r="K223" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L223" s="3" t="s">
         <v>22</v>
       </c>
@@ -10581,6 +11217,9 @@
       <c r="J224" s="3">
         <v>2</v>
       </c>
+      <c r="K224" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L224" s="3" t="s">
         <v>22</v>
       </c>
@@ -10622,6 +11261,9 @@
       <c r="J225" s="4">
         <v>2</v>
       </c>
+      <c r="K225" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L225" s="4" t="s">
         <v>22</v>
       </c>
@@ -10663,6 +11305,9 @@
       <c r="J226" s="3">
         <v>2</v>
       </c>
+      <c r="K226" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L226" s="3" t="s">
         <v>22</v>
       </c>
@@ -10704,6 +11349,9 @@
       <c r="J227" s="3">
         <v>2</v>
       </c>
+      <c r="K227" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L227" s="3" t="s">
         <v>22</v>
       </c>
@@ -10745,6 +11393,9 @@
       <c r="J228" s="3">
         <v>2</v>
       </c>
+      <c r="K228" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L228" s="3" t="s">
         <v>22</v>
       </c>
@@ -10786,6 +11437,9 @@
       <c r="J229" s="4">
         <v>2</v>
       </c>
+      <c r="K229" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L229" s="4" t="s">
         <v>22</v>
       </c>
@@ -10827,6 +11481,9 @@
       <c r="J230" s="3">
         <v>2</v>
       </c>
+      <c r="K230" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L230" s="3" t="s">
         <v>22</v>
       </c>
@@ -10868,6 +11525,9 @@
       <c r="J231" s="3">
         <v>2</v>
       </c>
+      <c r="K231" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L231" s="3" t="s">
         <v>22</v>
       </c>
@@ -10909,6 +11569,9 @@
       <c r="J232" s="3">
         <v>2</v>
       </c>
+      <c r="K232" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L232" s="3" t="s">
         <v>22</v>
       </c>
@@ -10950,6 +11613,9 @@
       <c r="J233" s="4">
         <v>2</v>
       </c>
+      <c r="K233" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L233" s="4" t="s">
         <v>22</v>
       </c>
@@ -10991,6 +11657,9 @@
       <c r="J234" s="3">
         <v>2</v>
       </c>
+      <c r="K234" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L234" s="3" t="s">
         <v>22</v>
       </c>
@@ -11032,6 +11701,9 @@
       <c r="J235" s="3">
         <v>2</v>
       </c>
+      <c r="K235" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L235" s="3" t="s">
         <v>22</v>
       </c>
@@ -11073,6 +11745,9 @@
       <c r="J236" s="3">
         <v>2</v>
       </c>
+      <c r="K236" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L236" s="3" t="s">
         <v>22</v>
       </c>
@@ -11114,6 +11789,9 @@
       <c r="J237" s="2">
         <v>2</v>
       </c>
+      <c r="K237" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L237" s="2" t="s">
         <v>22</v>
       </c>
@@ -11155,6 +11833,9 @@
       <c r="J238" s="3">
         <v>2</v>
       </c>
+      <c r="K238" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L238" s="3" t="s">
         <v>22</v>
       </c>
@@ -11196,6 +11877,9 @@
       <c r="J239" s="3">
         <v>2</v>
       </c>
+      <c r="K239" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L239" s="3" t="s">
         <v>22</v>
       </c>
@@ -11237,6 +11921,9 @@
       <c r="J240" s="3">
         <v>2</v>
       </c>
+      <c r="K240" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L240" s="3" t="s">
         <v>22</v>
       </c>
@@ -11278,6 +11965,9 @@
       <c r="J241" s="4">
         <v>2</v>
       </c>
+      <c r="K241" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L241" s="4" t="s">
         <v>22</v>
       </c>
@@ -11319,6 +12009,9 @@
       <c r="J242" s="3">
         <v>2</v>
       </c>
+      <c r="K242" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L242" s="3" t="s">
         <v>22</v>
       </c>
@@ -11360,6 +12053,9 @@
       <c r="J243" s="3">
         <v>2</v>
       </c>
+      <c r="K243" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L243" s="3" t="s">
         <v>22</v>
       </c>
@@ -11401,6 +12097,9 @@
       <c r="J244" s="3">
         <v>2</v>
       </c>
+      <c r="K244" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L244" s="3" t="s">
         <v>22</v>
       </c>
@@ -11442,6 +12141,9 @@
       <c r="J245" s="4">
         <v>2</v>
       </c>
+      <c r="K245" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L245" s="4" t="s">
         <v>22</v>
       </c>
@@ -11483,6 +12185,9 @@
       <c r="J246" s="3">
         <v>2</v>
       </c>
+      <c r="K246" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L246" s="3" t="s">
         <v>22</v>
       </c>
@@ -11524,6 +12229,9 @@
       <c r="J247" s="3">
         <v>2</v>
       </c>
+      <c r="K247" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L247" s="3" t="s">
         <v>22</v>
       </c>
@@ -11565,6 +12273,9 @@
       <c r="J248" s="3">
         <v>2</v>
       </c>
+      <c r="K248" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L248" s="3" t="s">
         <v>22</v>
       </c>
@@ -11606,6 +12317,9 @@
       <c r="J249" s="4">
         <v>2</v>
       </c>
+      <c r="K249" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L249" s="4" t="s">
         <v>22</v>
       </c>
@@ -11647,6 +12361,9 @@
       <c r="J250" s="3">
         <v>2</v>
       </c>
+      <c r="K250" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L250" s="3" t="s">
         <v>22</v>
       </c>
@@ -11688,6 +12405,9 @@
       <c r="J251" s="3">
         <v>2</v>
       </c>
+      <c r="K251" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L251" s="3" t="s">
         <v>22</v>
       </c>
@@ -11729,6 +12449,9 @@
       <c r="J252" s="3">
         <v>2</v>
       </c>
+      <c r="K252" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L252" s="3" t="s">
         <v>22</v>
       </c>
@@ -11770,6 +12493,9 @@
       <c r="J253" s="4">
         <v>2</v>
       </c>
+      <c r="K253" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L253" s="4" t="s">
         <v>22</v>
       </c>
@@ -11811,6 +12537,9 @@
       <c r="J254" s="3">
         <v>2</v>
       </c>
+      <c r="K254" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L254" s="3" t="s">
         <v>22</v>
       </c>
@@ -11852,6 +12581,9 @@
       <c r="J255" s="3">
         <v>2</v>
       </c>
+      <c r="K255" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L255" s="3" t="s">
         <v>22</v>
       </c>
@@ -11893,6 +12625,9 @@
       <c r="J256" s="3">
         <v>2</v>
       </c>
+      <c r="K256" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L256" s="3" t="s">
         <v>22</v>
       </c>
@@ -11934,6 +12669,9 @@
       <c r="J257" s="4">
         <v>2</v>
       </c>
+      <c r="K257" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L257" s="4" t="s">
         <v>22</v>
       </c>
@@ -11975,6 +12713,9 @@
       <c r="J258" s="3">
         <v>2</v>
       </c>
+      <c r="K258" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L258" s="3" t="s">
         <v>22</v>
       </c>
@@ -12016,6 +12757,9 @@
       <c r="J259" s="3">
         <v>2</v>
       </c>
+      <c r="K259" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L259" s="3" t="s">
         <v>22</v>
       </c>
@@ -12057,6 +12801,9 @@
       <c r="J260" s="3">
         <v>2</v>
       </c>
+      <c r="K260" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L260" s="3" t="s">
         <v>22</v>
       </c>
@@ -12098,6 +12845,9 @@
       <c r="J261" s="4">
         <v>2</v>
       </c>
+      <c r="K261" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L261" s="4" t="s">
         <v>22</v>
       </c>
@@ -12139,6 +12889,9 @@
       <c r="J262" s="3">
         <v>2</v>
       </c>
+      <c r="K262" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L262" s="3" t="s">
         <v>22</v>
       </c>
@@ -12180,6 +12933,9 @@
       <c r="J263" s="3">
         <v>2</v>
       </c>
+      <c r="K263" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L263" s="3" t="s">
         <v>22</v>
       </c>
@@ -12221,6 +12977,9 @@
       <c r="J264" s="3">
         <v>2</v>
       </c>
+      <c r="K264" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L264" s="3" t="s">
         <v>22</v>
       </c>
@@ -12262,6 +13021,9 @@
       <c r="J265" s="4">
         <v>2</v>
       </c>
+      <c r="K265" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L265" s="4" t="s">
         <v>22</v>
       </c>
@@ -12303,6 +13065,9 @@
       <c r="J266" s="3">
         <v>2</v>
       </c>
+      <c r="K266" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L266" s="3" t="s">
         <v>22</v>
       </c>
@@ -12344,6 +13109,9 @@
       <c r="J267" s="3">
         <v>2</v>
       </c>
+      <c r="K267" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L267" s="3" t="s">
         <v>22</v>
       </c>
@@ -12384,6 +13152,9 @@
       </c>
       <c r="J268" s="3">
         <v>2</v>
+      </c>
+      <c r="K268" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="L268" s="3" t="s">
         <v>22</v>
@@ -12426,6 +13197,9 @@
       <c r="J269" s="4">
         <v>4</v>
       </c>
+      <c r="K269" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L269" s="4" t="s">
         <v>22</v>
       </c>
@@ -12467,6 +13241,9 @@
       <c r="J270" s="3">
         <v>4</v>
       </c>
+      <c r="K270" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L270" s="3" t="s">
         <v>22</v>
       </c>
@@ -12508,6 +13285,9 @@
       <c r="J271" s="3">
         <v>4</v>
       </c>
+      <c r="K271" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L271" s="3" t="s">
         <v>22</v>
       </c>
@@ -12549,6 +13329,9 @@
       <c r="J272" s="3">
         <v>4</v>
       </c>
+      <c r="K272" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L272" s="3" t="s">
         <v>22</v>
       </c>
@@ -12590,6 +13373,9 @@
       <c r="J273" s="4">
         <v>4</v>
       </c>
+      <c r="K273" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L273" s="4" t="s">
         <v>22</v>
       </c>
@@ -12631,6 +13417,9 @@
       <c r="J274" s="3">
         <v>4</v>
       </c>
+      <c r="K274" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L274" s="3" t="s">
         <v>22</v>
       </c>
@@ -12672,6 +13461,9 @@
       <c r="J275" s="3">
         <v>4</v>
       </c>
+      <c r="K275" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L275" s="3" t="s">
         <v>22</v>
       </c>
@@ -12713,6 +13505,9 @@
       <c r="J276" s="3">
         <v>4</v>
       </c>
+      <c r="K276" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L276" s="3" t="s">
         <v>22</v>
       </c>
@@ -12754,6 +13549,9 @@
       <c r="J277" s="4">
         <v>2</v>
       </c>
+      <c r="K277" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L277" s="4" t="s">
         <v>22</v>
       </c>
@@ -12795,6 +13593,9 @@
       <c r="J278" s="3">
         <v>2</v>
       </c>
+      <c r="K278" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L278" s="3" t="s">
         <v>22</v>
       </c>
@@ -12836,6 +13637,9 @@
       <c r="J279" s="3">
         <v>2</v>
       </c>
+      <c r="K279" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L279" s="3" t="s">
         <v>22</v>
       </c>
@@ -12877,6 +13681,9 @@
       <c r="J280" s="3">
         <v>2</v>
       </c>
+      <c r="K280" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L280" s="3" t="s">
         <v>22</v>
       </c>
@@ -12918,6 +13725,9 @@
       <c r="J281" s="4">
         <v>2</v>
       </c>
+      <c r="K281" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L281" s="4" t="s">
         <v>22</v>
       </c>
@@ -12959,6 +13769,9 @@
       <c r="J282" s="3">
         <v>2</v>
       </c>
+      <c r="K282" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L282" s="3" t="s">
         <v>22</v>
       </c>
@@ -13000,6 +13813,9 @@
       <c r="J283" s="3">
         <v>2</v>
       </c>
+      <c r="K283" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L283" s="3" t="s">
         <v>22</v>
       </c>
@@ -13041,6 +13857,9 @@
       <c r="J284" s="3">
         <v>2</v>
       </c>
+      <c r="K284" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L284" s="3" t="s">
         <v>22</v>
       </c>
@@ -13082,6 +13901,9 @@
       <c r="J285" s="4">
         <v>2</v>
       </c>
+      <c r="K285" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L285" s="4" t="s">
         <v>22</v>
       </c>
@@ -13123,6 +13945,9 @@
       <c r="J286" s="3">
         <v>2</v>
       </c>
+      <c r="K286" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L286" s="3" t="s">
         <v>22</v>
       </c>
@@ -13164,6 +13989,9 @@
       <c r="J287" s="3">
         <v>2</v>
       </c>
+      <c r="K287" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L287" s="3" t="s">
         <v>22</v>
       </c>
@@ -13205,6 +14033,9 @@
       <c r="J288" s="3">
         <v>2</v>
       </c>
+      <c r="K288" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L288" s="3" t="s">
         <v>22</v>
       </c>
@@ -13246,6 +14077,9 @@
       <c r="J289" s="4">
         <v>2</v>
       </c>
+      <c r="K289" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L289" s="4" t="s">
         <v>22</v>
       </c>
@@ -13287,6 +14121,9 @@
       <c r="J290" s="3">
         <v>2</v>
       </c>
+      <c r="K290" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L290" s="3" t="s">
         <v>22</v>
       </c>
@@ -13328,6 +14165,9 @@
       <c r="J291" s="3">
         <v>2</v>
       </c>
+      <c r="K291" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L291" s="3" t="s">
         <v>22</v>
       </c>
@@ -13369,6 +14209,9 @@
       <c r="J292" s="3">
         <v>2</v>
       </c>
+      <c r="K292" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L292" s="3" t="s">
         <v>22</v>
       </c>
@@ -13408,6 +14251,9 @@
       <c r="J293" s="4">
         <v>2</v>
       </c>
+      <c r="K293" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L293" s="4" t="s">
         <v>22</v>
       </c>
@@ -13447,6 +14293,9 @@
       <c r="J294" s="3">
         <v>2</v>
       </c>
+      <c r="K294" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L294" s="3" t="s">
         <v>22</v>
       </c>
@@ -13486,6 +14335,9 @@
       <c r="J295" s="3">
         <v>2</v>
       </c>
+      <c r="K295" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L295" s="3" t="s">
         <v>22</v>
       </c>
@@ -13525,6 +14377,9 @@
       <c r="J296" s="3">
         <v>2</v>
       </c>
+      <c r="K296" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L296" s="3" t="s">
         <v>22</v>
       </c>
@@ -13566,6 +14421,9 @@
       <c r="J297" s="4">
         <v>1</v>
       </c>
+      <c r="K297" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L297" s="4" t="s">
         <v>22</v>
       </c>
@@ -13607,6 +14465,9 @@
       <c r="J298" s="3">
         <v>1</v>
       </c>
+      <c r="K298" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L298" s="3" t="s">
         <v>22</v>
       </c>
@@ -13648,6 +14509,9 @@
       <c r="J299" s="3">
         <v>1</v>
       </c>
+      <c r="K299" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L299" s="3" t="s">
         <v>22</v>
       </c>
@@ -13689,6 +14553,9 @@
       <c r="J300" s="3">
         <v>1</v>
       </c>
+      <c r="K300" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L300" s="3" t="s">
         <v>22</v>
       </c>
@@ -13730,6 +14597,9 @@
       <c r="J301" s="4">
         <v>3</v>
       </c>
+      <c r="K301" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L301" s="4" t="s">
         <v>22</v>
       </c>
@@ -13771,6 +14641,9 @@
       <c r="J302" s="3">
         <v>3</v>
       </c>
+      <c r="K302" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L302" s="3" t="s">
         <v>22</v>
       </c>
@@ -13812,6 +14685,9 @@
       <c r="J303" s="3">
         <v>3</v>
       </c>
+      <c r="K303" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L303" s="3" t="s">
         <v>22</v>
       </c>
@@ -13853,6 +14729,9 @@
       <c r="J304" s="3">
         <v>3</v>
       </c>
+      <c r="K304" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L304" s="3" t="s">
         <v>22</v>
       </c>
@@ -13894,6 +14773,9 @@
       <c r="J305" s="3">
         <v>3</v>
       </c>
+      <c r="K305" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L305" s="3" t="s">
         <v>22</v>
       </c>
@@ -13935,6 +14817,9 @@
       <c r="J306" s="3">
         <v>3</v>
       </c>
+      <c r="K306" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L306" s="3" t="s">
         <v>22</v>
       </c>
@@ -13976,6 +14861,9 @@
       <c r="J307" s="3">
         <v>3</v>
       </c>
+      <c r="K307" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L307" s="3" t="s">
         <v>22</v>
       </c>
@@ -14017,6 +14905,9 @@
       <c r="J308" s="3">
         <v>3</v>
       </c>
+      <c r="K308" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L308" s="3" t="s">
         <v>22</v>
       </c>
@@ -14058,6 +14949,9 @@
       <c r="J309" s="4">
         <v>1</v>
       </c>
+      <c r="K309" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L309" s="4" t="s">
         <v>22</v>
       </c>
@@ -14099,6 +14993,9 @@
       <c r="J310" s="3">
         <v>1</v>
       </c>
+      <c r="K310" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L310" s="3" t="s">
         <v>22</v>
       </c>
@@ -14140,6 +15037,9 @@
       <c r="J311" s="3">
         <v>1</v>
       </c>
+      <c r="K311" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L311" s="3" t="s">
         <v>22</v>
       </c>
@@ -14181,6 +15081,9 @@
       <c r="J312" s="3">
         <v>1</v>
       </c>
+      <c r="K312" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L312" s="3" t="s">
         <v>22</v>
       </c>
@@ -14222,6 +15125,9 @@
       <c r="J313" s="4">
         <v>3</v>
       </c>
+      <c r="K313" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L313" s="4" t="s">
         <v>22</v>
       </c>
@@ -14263,6 +15169,9 @@
       <c r="J314" s="3">
         <v>3</v>
       </c>
+      <c r="K314" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L314" s="3" t="s">
         <v>22</v>
       </c>
@@ -14304,6 +15213,9 @@
       <c r="J315" s="3">
         <v>3</v>
       </c>
+      <c r="K315" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L315" s="3" t="s">
         <v>22</v>
       </c>
@@ -14345,6 +15257,9 @@
       <c r="J316" s="3">
         <v>3</v>
       </c>
+      <c r="K316" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L316" s="3" t="s">
         <v>22</v>
       </c>
@@ -14386,6 +15301,9 @@
       <c r="J317" s="3">
         <v>3</v>
       </c>
+      <c r="K317" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L317" s="3" t="s">
         <v>22</v>
       </c>
@@ -14427,6 +15345,9 @@
       <c r="J318" s="3">
         <v>3</v>
       </c>
+      <c r="K318" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L318" s="3" t="s">
         <v>22</v>
       </c>
@@ -14468,6 +15389,9 @@
       <c r="J319" s="3">
         <v>3</v>
       </c>
+      <c r="K319" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L319" s="3" t="s">
         <v>22</v>
       </c>
@@ -14508,6 +15432,9 @@
       </c>
       <c r="J320" s="3">
         <v>3</v>
+      </c>
+      <c r="K320" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="L320" s="3" t="s">
         <v>22</v>
@@ -14548,6 +15475,9 @@
       <c r="J321" s="2">
         <v>32</v>
       </c>
+      <c r="K321" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L321" s="2" t="s">
         <v>22</v>
       </c>
@@ -14587,6 +15517,9 @@
       <c r="J322" s="4">
         <v>32</v>
       </c>
+      <c r="K322" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L322" s="4" t="s">
         <v>22</v>
       </c>
@@ -14628,6 +15561,9 @@
       <c r="J323" s="2">
         <v>32</v>
       </c>
+      <c r="K323" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L323" s="2" t="s">
         <v>22</v>
       </c>
@@ -14669,6 +15605,9 @@
       <c r="J324" s="4">
         <v>32</v>
       </c>
+      <c r="K324" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L324" s="4" t="s">
         <v>22</v>
       </c>
@@ -14710,6 +15649,9 @@
       <c r="J325" s="2">
         <v>32</v>
       </c>
+      <c r="K325" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L325" s="2" t="s">
         <v>22</v>
       </c>
@@ -14751,6 +15693,9 @@
       <c r="J326" s="4">
         <v>32</v>
       </c>
+      <c r="K326" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L326" s="4" t="s">
         <v>22</v>
       </c>
@@ -14792,6 +15737,9 @@
       <c r="J327" s="2">
         <v>16</v>
       </c>
+      <c r="K327" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L327" s="2" t="s">
         <v>22</v>
       </c>
@@ -14833,6 +15781,9 @@
       <c r="J328" s="4">
         <v>16</v>
       </c>
+      <c r="K328" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L328" s="4" t="s">
         <v>22</v>
       </c>
@@ -14874,6 +15825,9 @@
       <c r="J329" s="2">
         <v>16</v>
       </c>
+      <c r="K329" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L329" s="2" t="s">
         <v>22</v>
       </c>
@@ -14915,6 +15869,9 @@
       <c r="J330" s="4">
         <v>16</v>
       </c>
+      <c r="K330" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L330" s="4" t="s">
         <v>22</v>
       </c>
@@ -14956,6 +15913,9 @@
       <c r="J331" s="4">
         <v>16</v>
       </c>
+      <c r="K331" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L331" s="4" t="s">
         <v>22</v>
       </c>
@@ -14995,6 +15955,9 @@
       <c r="J332" s="2">
         <v>16</v>
       </c>
+      <c r="K332" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L332" s="2" t="s">
         <v>22</v>
       </c>
@@ -15034,6 +15997,9 @@
       <c r="J333" s="4">
         <v>16</v>
       </c>
+      <c r="K333" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L333" s="4" t="s">
         <v>22</v>
       </c>
@@ -15073,6 +16039,9 @@
       <c r="J334" s="4">
         <v>16</v>
       </c>
+      <c r="K334" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L334" s="4" t="s">
         <v>22</v>
       </c>
@@ -15112,6 +16081,9 @@
       <c r="J335" s="2">
         <v>16</v>
       </c>
+      <c r="K335" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L335" s="2" t="s">
         <v>22</v>
       </c>
@@ -15151,6 +16123,9 @@
       <c r="J336" s="4">
         <v>16</v>
       </c>
+      <c r="K336" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L336" s="4" t="s">
         <v>22</v>
       </c>
@@ -15189,6 +16164,9 @@
       </c>
       <c r="J337" s="4">
         <v>16</v>
+      </c>
+      <c r="K337" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="L337" s="4" t="s">
         <v>22</v>
@@ -15647,6 +16625,9 @@
       <c r="J348" s="4">
         <v>16</v>
       </c>
+      <c r="K348" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L348" s="4" t="s">
         <v>22</v>
       </c>
@@ -15684,6 +16665,9 @@
       <c r="J349" s="4">
         <v>16</v>
       </c>
+      <c r="K349" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L349" s="4" t="s">
         <v>22</v>
       </c>
@@ -15723,6 +16707,9 @@
       <c r="J350" s="4">
         <v>16</v>
       </c>
+      <c r="K350" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L350" s="4" t="s">
         <v>22</v>
       </c>
@@ -15762,6 +16749,9 @@
       <c r="J351" s="4">
         <v>16</v>
       </c>
+      <c r="K351" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L351" s="4" t="s">
         <v>22</v>
       </c>
@@ -15801,6 +16791,9 @@
       <c r="J352" s="4">
         <v>16</v>
       </c>
+      <c r="K352" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L352" s="4" t="s">
         <v>22</v>
       </c>
@@ -15840,6 +16833,9 @@
       <c r="J353" s="4">
         <v>16</v>
       </c>
+      <c r="K353" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L353" s="4" t="s">
         <v>22</v>
       </c>
@@ -15879,6 +16875,9 @@
       <c r="J354" s="4">
         <v>8</v>
       </c>
+      <c r="K354" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L354" s="4" t="s">
         <v>22</v>
       </c>
@@ -15916,6 +16915,9 @@
       <c r="J355" s="4">
         <v>16</v>
       </c>
+      <c r="K355" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L355" s="4" t="s">
         <v>22</v>
       </c>
@@ -15953,6 +16955,9 @@
       <c r="J356" s="4">
         <v>16</v>
       </c>
+      <c r="K356" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L356" s="4" t="s">
         <v>22</v>
       </c>
@@ -15992,6 +16997,9 @@
       <c r="J357" s="4">
         <v>2</v>
       </c>
+      <c r="K357" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L357" s="4" t="s">
         <v>22</v>
       </c>
@@ -16031,6 +17039,9 @@
       <c r="J358" s="3">
         <v>2</v>
       </c>
+      <c r="K358" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L358" s="3" t="s">
         <v>22</v>
       </c>
@@ -16070,6 +17081,9 @@
       <c r="J359" s="3">
         <v>2</v>
       </c>
+      <c r="K359" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L359" s="3" t="s">
         <v>22</v>
       </c>
@@ -16109,6 +17123,9 @@
       <c r="J360" s="3">
         <v>2</v>
       </c>
+      <c r="K360" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L360" s="3" t="s">
         <v>22</v>
       </c>
@@ -16148,6 +17165,9 @@
       <c r="J361" s="4">
         <v>8</v>
       </c>
+      <c r="K361" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L361" s="4" t="s">
         <v>22</v>
       </c>
@@ -16185,6 +17205,9 @@
       <c r="J362" s="4">
         <v>16</v>
       </c>
+      <c r="K362" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L362" s="4" t="s">
         <v>22</v>
       </c>
@@ -16224,6 +17247,9 @@
       <c r="J363" s="4">
         <v>4</v>
       </c>
+      <c r="K363" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L363" s="4" t="s">
         <v>22</v>
       </c>
@@ -16263,6 +17289,9 @@
       <c r="J364" s="3">
         <v>4</v>
       </c>
+      <c r="K364" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L364" s="3" t="s">
         <v>22</v>
       </c>
@@ -16302,6 +17331,9 @@
       <c r="J365" s="3">
         <v>4</v>
       </c>
+      <c r="K365" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L365" s="3" t="s">
         <v>22</v>
       </c>
@@ -16341,6 +17373,9 @@
       <c r="J366" s="3">
         <v>4</v>
       </c>
+      <c r="K366" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="L366" s="3" t="s">
         <v>22</v>
       </c>
@@ -16380,6 +17415,9 @@
       <c r="J367" s="4">
         <v>16</v>
       </c>
+      <c r="K367" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L367" s="4" t="s">
         <v>22</v>
       </c>
@@ -16419,6 +17457,9 @@
       <c r="J368" s="4">
         <v>16</v>
       </c>
+      <c r="K368" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L368" s="4" t="s">
         <v>22</v>
       </c>
@@ -16458,6 +17499,9 @@
       <c r="J369" s="4">
         <v>16</v>
       </c>
+      <c r="K369" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L369" s="4" t="s">
         <v>22</v>
       </c>
@@ -16497,6 +17541,9 @@
       <c r="J370" s="4">
         <v>16</v>
       </c>
+      <c r="K370" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L370" s="4" t="s">
         <v>22</v>
       </c>
@@ -16536,6 +17583,9 @@
       <c r="J371" s="4">
         <v>16</v>
       </c>
+      <c r="K371" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L371" s="4" t="s">
         <v>22</v>
       </c>
@@ -16575,6 +17625,9 @@
       <c r="J372" s="4">
         <v>16</v>
       </c>
+      <c r="K372" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L372" s="4" t="s">
         <v>22</v>
       </c>
@@ -16614,6 +17667,9 @@
       <c r="J373" s="4">
         <v>16</v>
       </c>
+      <c r="K373" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L373" s="4" t="s">
         <v>22</v>
       </c>
@@ -16653,6 +17709,9 @@
       <c r="J374" s="4">
         <v>16</v>
       </c>
+      <c r="K374" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L374" s="4" t="s">
         <v>22</v>
       </c>
@@ -16690,6 +17749,9 @@
       <c r="J375" s="4">
         <v>16</v>
       </c>
+      <c r="K375" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L375" s="4" t="s">
         <v>22</v>
       </c>
@@ -16729,6 +17791,9 @@
       <c r="J376" s="2">
         <v>32</v>
       </c>
+      <c r="K376" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L376" s="2" t="s">
         <v>22</v>
       </c>
@@ -16768,6 +17833,9 @@
       <c r="J377" s="2">
         <v>16</v>
       </c>
+      <c r="K377" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L377" s="2" t="s">
         <v>22</v>
       </c>
@@ -16807,6 +17875,9 @@
       <c r="J378" s="4">
         <v>16</v>
       </c>
+      <c r="K378" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L378" s="4" t="s">
         <v>22</v>
       </c>
@@ -16846,6 +17917,9 @@
       <c r="J379" s="4">
         <v>32</v>
       </c>
+      <c r="K379" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L379" s="4" t="s">
         <v>22</v>
       </c>
@@ -16885,6 +17959,9 @@
       <c r="J380" s="2">
         <v>16</v>
       </c>
+      <c r="K380" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L380" s="2" t="s">
         <v>22</v>
       </c>
@@ -16926,6 +18003,9 @@
       <c r="J381" s="4">
         <v>16</v>
       </c>
+      <c r="K381" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L381" s="4" t="s">
         <v>22</v>
       </c>
@@ -16967,6 +18047,9 @@
       <c r="J382" s="4">
         <v>16</v>
       </c>
+      <c r="K382" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L382" s="4" t="s">
         <v>22</v>
       </c>
@@ -17008,6 +18091,9 @@
       <c r="J383" s="4">
         <v>16</v>
       </c>
+      <c r="K383" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L383" s="4" t="s">
         <v>22</v>
       </c>
@@ -17049,6 +18135,9 @@
       <c r="J384" s="2">
         <v>16</v>
       </c>
+      <c r="K384" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L384" s="2" t="s">
         <v>22</v>
       </c>
@@ -17090,6 +18179,9 @@
       <c r="J385" s="4">
         <v>16</v>
       </c>
+      <c r="K385" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L385" s="4" t="s">
         <v>22</v>
       </c>
@@ -17129,6 +18221,9 @@
       <c r="J386" s="4">
         <v>16</v>
       </c>
+      <c r="K386" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L386" s="4" t="s">
         <v>22</v>
       </c>
@@ -17168,6 +18263,9 @@
       <c r="J387" s="2">
         <v>16</v>
       </c>
+      <c r="K387" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L387" s="2" t="s">
         <v>22</v>
       </c>
@@ -17209,6 +18307,9 @@
       <c r="J388" s="4">
         <v>16</v>
       </c>
+      <c r="K388" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="L388" s="4" t="s">
         <v>22</v>
       </c>
@@ -17249,6 +18350,9 @@
       </c>
       <c r="J389" s="4">
         <v>16</v>
+      </c>
+      <c r="K389" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="L389" s="4" t="s">
         <v>22</v>
@@ -17289,6 +18393,9 @@
       <c r="J390" s="2">
         <v>32</v>
       </c>
+      <c r="K390" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L390" s="2" t="s">
         <v>22</v>
       </c>
@@ -17326,6 +18433,9 @@
       <c r="J391" s="2">
         <v>28</v>
       </c>
+      <c r="K391" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="L391" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>